<commit_message>
sort column and format code
</commit_message>
<xml_diff>
--- a/src/export/bill.xlsx
+++ b/src/export/bill.xlsx
@@ -1,19 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GIT\MINORI\newtransport\newstransport-cms-api\src\export\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9341FD-F518-4A2F-BDA6-F34485840148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Danh sách vận đơn" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,36 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Mã vận đơn</t>
+  </si>
   <si>
     <t>Mã khách hàng</t>
   </si>
   <si>
-    <t>Tên người gửi</t>
-  </si>
-  <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>TT kế toán</t>
-  </si>
-  <si>
-    <t>Tỉnh/Thành bên chuyển</t>
-  </si>
-  <si>
-    <t>Quận/Huyện bên chuyển</t>
-  </si>
-  <si>
-    <t>Tỉnh/Thành bên phát</t>
-  </si>
-  <si>
-    <t>Quận/Huyện bên phát</t>
-  </si>
-  <si>
-    <t>Nhân viên thực hiện</t>
-  </si>
-  <si>
-    <t>Nhân viên vận chuyển</t>
+    <t>Tên khách hàng</t>
+  </si>
+  <si>
+    <t>Tỉnh/Thành nhận</t>
+  </si>
+  <si>
+    <t>Quận/Huyện nhận</t>
+  </si>
+  <si>
+    <t>Tỉnh/Thành phát</t>
+  </si>
+  <si>
+    <t>Quận/Huyện phát</t>
+  </si>
+  <si>
+    <t>Trạng thái kế toán</t>
+  </si>
+  <si>
+    <t>Nhân viên phát</t>
   </si>
   <si>
     <t>Trạng thái tồn</t>
@@ -66,43 +57,25 @@
     <t>Dịch vụ cộng thêm 1</t>
   </si>
   <si>
-    <t>Dịch vụ cộng thêm 2</t>
-  </si>
-  <si>
-    <t>Dịch vụ cộng thêm 3</t>
-  </si>
-  <si>
-    <t>Dịch vụ cộng thêm 4</t>
-  </si>
-  <si>
-    <t>Dịch vụ cộng thêm 5</t>
-  </si>
-  <si>
-    <t>Trọng lượng</t>
-  </si>
-  <si>
-    <t>Đơn vị trọng lượng</t>
-  </si>
-  <si>
-    <t>Loại xe</t>
+    <t>Trọng lượng Kg/Tấn/Khối</t>
+  </si>
+  <si>
+    <t>Loại phương tiện</t>
+  </si>
+  <si>
+    <t>Nội dung hàng hóa</t>
+  </si>
+  <si>
+    <t>Trạng thái vận chuyển</t>
   </si>
   <si>
     <t>Chiết khấu</t>
   </si>
   <si>
-    <t>Đơn vị chiết khấu</t>
-  </si>
-  <si>
-    <t>Tổng cước (VND)</t>
-  </si>
-  <si>
-    <t>Hàng hóa</t>
-  </si>
-  <si>
-    <t>Địa chỉ người gửi</t>
-  </si>
-  <si>
-    <t>Số DT người gửi</t>
+    <t>Tổng cước</t>
+  </si>
+  <si>
+    <t>Địa chỉ khách hàng</t>
   </si>
   <si>
     <t>Tên người nhận</t>
@@ -111,32 +84,20 @@
     <t>Địa chỉ người nhận</t>
   </si>
   <si>
-    <t xml:space="preserve">Số DT người nhận </t>
-  </si>
-  <si>
-    <t>Thời gian tạo</t>
-  </si>
-  <si>
-    <t>Mã đơn hàng 1</t>
+    <t>Thời gian nhận vận đơn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -147,7 +108,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -161,18 +122,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -190,6 +151,32 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -197,29 +184,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,121 +485,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="23" width="18.7109375" style="1"/>
-    <col min="24" max="24" width="18.7109375" style="6"/>
-    <col min="25" max="16384" width="18.7109375" style="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
     </row>
-    <row r="2" spans="1:31" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="9"/>
-      <c r="X2" s="5"/>
+    <row r="2" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update template and column
</commit_message>
<xml_diff>
--- a/src/export/bill.xlsx
+++ b/src/export/bill.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Mã vận đơn</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Thời gian nhận vận đơn</t>
+  </si>
+  <si>
+    <t>Dịch vụ cộng thêm 2</t>
+  </si>
+  <si>
+    <t>Dịch vụ cộng thêm 3</t>
+  </si>
+  <si>
+    <t>Dịch vụ cộng thêm 4</t>
+  </si>
+  <si>
+    <t>Dịch vụ cộng thêm 5</t>
+  </si>
+  <si>
+    <t>Nhân viên nhận</t>
   </si>
 </sst>
 </file>
@@ -486,11 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -498,7 +513,7 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -528,49 +543,64 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
     </row>
-    <row r="2" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
@@ -584,15 +614,20 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="7"/>
       <c r="W2" s="6"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>